<commit_message>
demos: fixed stroop builder demo - it was using wrong keys in trialList
</commit_message>
<xml_diff>
--- a/psychopy/demos/builder/stroop/trialTypes.xlsx
+++ b/psychopy/demos/builder/stroop/trialTypes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="-20" windowWidth="29600" windowHeight="18460" tabRatio="500"/>
+    <workbookView xWindow="-20" yWindow="-20" windowWidth="21600" windowHeight="13760" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="trialTypes.csv" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="10">
   <si>
     <t>letterColor</t>
   </si>
@@ -40,6 +40,18 @@
   </si>
   <si>
     <t>text</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>left</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>down</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>right</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -412,7 +424,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -438,8 +450,8 @@
       <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="C2">
-        <v>1</v>
+      <c r="C2" t="s">
+        <v>7</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -452,8 +464,8 @@
       <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="C3">
-        <v>2</v>
+      <c r="C3" t="s">
+        <v>8</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -466,8 +478,8 @@
       <c r="B4" t="s">
         <v>4</v>
       </c>
-      <c r="C4">
-        <v>2</v>
+      <c r="C4" t="s">
+        <v>8</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -480,8 +492,8 @@
       <c r="B5" t="s">
         <v>5</v>
       </c>
-      <c r="C5">
-        <v>3</v>
+      <c r="C5" t="s">
+        <v>9</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -494,8 +506,8 @@
       <c r="B6" t="s">
         <v>5</v>
       </c>
-      <c r="C6">
-        <v>3</v>
+      <c r="C6" t="s">
+        <v>9</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -508,15 +520,14 @@
       <c r="B7" t="s">
         <v>3</v>
       </c>
-      <c r="C7">
-        <v>1</v>
+      <c r="C7" t="s">
+        <v>7</v>
       </c>
       <c r="D7">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>